<commit_message>
atualização goleiro caio e jogador caio
</commit_message>
<xml_diff>
--- a/pelada_sabado_02_semestre.xlsx
+++ b/pelada_sabado_02_semestre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Fernando.Resende\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8F71BC-48D9-4D2C-B8C9-D505FB2DC48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF4A460-B3CA-4907-AF52-36D7473DA2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="62">
   <si>
     <t>Boneco</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Marmita</t>
+  </si>
+  <si>
+    <t>Caio Goleiro</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K200" sqref="K200"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1956,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C45">
         <v>4</v>

</xml_diff>